<commit_message>
Add Upgrade option for properties
</commit_message>
<xml_diff>
--- a/_Data/Properties-Detail.xlsx
+++ b/_Data/Properties-Detail.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="55">
   <si>
     <t>index</t>
   </si>
@@ -40,15 +40,18 @@
     <t>stay_place</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Salvador</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
     <t>Brazil</t>
   </si>
   <si>
-    <t>Salvador</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
     <t>Chance</t>
   </si>
   <si>
@@ -148,12 +151,12 @@
     <t>Auction (Trade)</t>
   </si>
   <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
     <t>England</t>
   </si>
   <si>
-    <t>Liverpool</t>
-  </si>
-  <si>
     <t>Manchester</t>
   </si>
   <si>
@@ -163,10 +166,10 @@
     <t>Airport 2</t>
   </si>
   <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
     <t>USA</t>
-  </si>
-  <si>
-    <t>Los Angeles</t>
   </si>
   <si>
     <t>San Francisco</t>
@@ -647,13 +650,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1">
         <v>60</v>
       </c>
       <c r="F3" s="1">
-        <f>(30/100)*E3</f>
+        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -661,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
@@ -673,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <f>(30/100)*E4</f>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -681,19 +684,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1">
         <v>70</v>
       </c>
       <c r="F5" s="1">
-        <f>(30/100)*E5</f>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -701,7 +704,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -713,7 +716,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <f>(30/100)*E6</f>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -721,19 +724,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1">
         <v>70</v>
       </c>
       <c r="F7" s="1">
-        <f>(30/100)*E7</f>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -741,19 +744,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1">
         <v>150</v>
       </c>
       <c r="F8" s="1">
-        <f>(30/100)*E8</f>
+        <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -761,19 +764,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1">
         <v>90</v>
       </c>
       <c r="F9" s="1">
-        <f>(30/100)*E9</f>
+        <v>27</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
@@ -781,19 +784,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1">
         <v>80</v>
       </c>
       <c r="F10" s="1">
-        <f>(30/100)*E10</f>
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
@@ -801,19 +804,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <f>(30/100)*E11</f>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
@@ -821,19 +824,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="1">
         <v>100</v>
       </c>
       <c r="F12" s="1">
-        <f>(30/100)*E12</f>
+        <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
@@ -841,19 +844,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1">
         <v>150</v>
       </c>
       <c r="F13" s="1">
-        <f>(30/100)*E13</f>
+        <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
@@ -861,19 +864,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1">
         <v>110</v>
       </c>
       <c r="F14" s="1">
-        <f>(30/100)*E14</f>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
@@ -881,19 +884,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1">
         <v>100</v>
       </c>
       <c r="F15" s="1">
-        <f>(30/100)*E15</f>
+        <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
@@ -901,19 +904,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1">
         <v>200</v>
       </c>
       <c r="F16" s="1">
-        <f>(30/100)*E16</f>
+        <v>60</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
@@ -921,19 +924,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E17" s="1">
         <v>120</v>
       </c>
       <c r="F17" s="1">
-        <f>(30/100)*E17</f>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
@@ -941,19 +944,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
       </c>
       <c r="F18" s="1">
-        <f>(30/100)*E18</f>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
@@ -961,19 +964,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E19" s="1">
         <v>170</v>
       </c>
       <c r="F19" s="1">
-        <f>(30/100)*E19</f>
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
@@ -981,19 +984,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E20" s="1">
         <v>150</v>
       </c>
       <c r="F20" s="1">
-        <f>(30/100)*E20</f>
+        <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
@@ -1001,19 +1004,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="1">
-        <f>(30/100)*E21</f>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
@@ -1021,19 +1024,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E22" s="1">
         <v>210</v>
       </c>
       <c r="F22" s="1">
-        <f>(30/100)*E22</f>
+        <v>63</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
@@ -1041,19 +1044,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
       </c>
       <c r="F23" s="1">
-        <f>(30/100)*E23</f>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
@@ -1061,19 +1064,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E24" s="1">
         <v>190</v>
       </c>
       <c r="F24" s="1">
-        <f>(30/100)*E24</f>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
@@ -1081,19 +1084,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E25" s="1">
         <v>180</v>
       </c>
       <c r="F25" s="1">
-        <f>(30/100)*E25</f>
+        <v>54</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
@@ -1101,19 +1104,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
       </c>
       <c r="F26" s="1">
-        <f>(30/100)*E26</f>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
@@ -1121,19 +1124,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E27" s="1">
         <v>220</v>
       </c>
       <c r="F27" s="1">
-        <f>(30/100)*E27</f>
+        <v>66</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
@@ -1141,19 +1144,19 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="E28" s="1">
         <v>240</v>
       </c>
       <c r="F28" s="1">
-        <f>(30/100)*E28</f>
+        <v>72</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
@@ -1161,19 +1164,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1">
         <v>200</v>
       </c>
       <c r="F29" s="1">
-        <f>(30/100)*E29</f>
+        <v>60</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25">
@@ -1181,19 +1184,19 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E30" s="1">
         <v>250</v>
       </c>
       <c r="F30" s="1">
-        <f>(30/100)*E30</f>
+        <v>75</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25">
@@ -1201,19 +1204,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
       <c r="F31" s="1">
-        <f>(30/100)*E31</f>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25">
@@ -1221,19 +1224,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
       <c r="F32" s="1">
-        <f>(30/100)*E32</f>
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25">
@@ -1247,13 +1250,13 @@
         <v>10</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E33" s="1">
         <v>280</v>
       </c>
       <c r="F33" s="1">
-        <f>(30/100)*E33</f>
+        <v>84</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="20.25">
@@ -1261,19 +1264,19 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="E34" s="1">
         <v>300</v>
       </c>
       <c r="F34" s="1">
-        <f>(30/100)*E34</f>
+        <v>90</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25">
@@ -1281,62 +1284,62 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="1">
-        <f>(30/100)*E35</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E36" s="1">
         <v>320</v>
       </c>
       <c r="F36" s="1">
-        <f>(30/100)*E36</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+        <v>96</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E37" s="1">
         <v>200</v>
       </c>
       <c r="F37" s="1">
-        <f>(30/100)*E37</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+        <v>60</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="20.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1347,13 +1350,13 @@
         <v>10</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E38" s="1">
         <v>320</v>
       </c>
       <c r="F38" s="1">
-        <f>(30/100)*E38</f>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
@@ -1361,19 +1364,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="E39" s="1">
         <v>350</v>
       </c>
       <c r="F39" s="1">
-        <f>(30/100)*E39</f>
+        <v>105</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
@@ -1381,19 +1384,19 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E40" s="1">
         <v>100</v>
       </c>
       <c r="F40" s="1">
-        <f>(30/100)*E40</f>
+        <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
@@ -1401,19 +1404,19 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E41" s="1">
         <v>380</v>
       </c>
       <c r="F41" s="1">
-        <f>(30/100)*E41</f>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last cleanings before submitting AI project...
</commit_message>
<xml_diff>
--- a/_Data/Properties-Detail.xlsx
+++ b/_Data/Properties-Detail.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProgramingProjects\Python\Monopoly Game\_Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7231746-4CC6-4E5D-BB12-A5D1FC8628D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -184,8 +190,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,7 +206,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,7 +215,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFe2f0d9"/>
+        <fgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -231,16 +242,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -248,52 +259,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:F41" displayName="Table1" name="Table1" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:F41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F41" totalsRowShown="0">
+  <autoFilter ref="A1:F41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn name="index" id="1"/>
-    <tableColumn name="place" id="2"/>
-    <tableColumn name="type" id="3"/>
-    <tableColumn name="country" id="4"/>
-    <tableColumn name="price" id="5"/>
-    <tableColumn name="rent" id="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="index"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="place"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="type"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="country"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="price"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="rent"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="0" showLastColumn="0" showFirstColumn="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -302,10 +322,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -343,71 +363,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,7 +455,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -458,11 +478,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -471,13 +491,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -487,7 +507,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -496,7 +516,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -505,7 +525,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -513,10 +533,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -581,25 +601,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="19.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="8.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,7 +641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -629,7 +651,7 @@
       <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3">
@@ -639,7 +661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -659,7 +681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row r="4" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -679,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row r="5" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -699,7 +721,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row r="6" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -719,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -739,7 +761,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+    <row r="8" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -759,7 +781,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+    <row r="9" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -779,7 +801,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+    <row r="10" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -799,7 +821,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
+    <row r="11" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -809,17 +831,17 @@
       <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -839,7 +861,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
+    <row r="13" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -859,7 +881,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
+    <row r="14" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -879,7 +901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+    <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -899,7 +921,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+    <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -919,7 +941,7 @@
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+    <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -939,7 +961,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
+    <row r="18" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -959,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
+    <row r="19" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -979,7 +1001,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
+    <row r="20" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -999,7 +1021,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
+    <row r="21" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1009,17 +1031,17 @@
       <c r="C21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
-      <c r="F21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
+      <c r="F21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1039,7 +1061,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
+    <row r="23" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1059,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
+    <row r="24" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1079,7 +1101,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
+    <row r="25" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1099,7 +1121,7 @@
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
+    <row r="26" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1119,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
+    <row r="27" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1139,7 +1161,7 @@
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
+    <row r="28" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1159,7 +1181,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
+    <row r="29" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1179,7 +1201,7 @@
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25">
+    <row r="30" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1199,7 +1221,7 @@
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25">
+    <row r="31" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -1209,17 +1231,17 @@
       <c r="C31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
       </c>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25">
+      <c r="F31" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1239,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25">
+    <row r="33" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1259,7 +1281,7 @@
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="20.25">
+    <row r="34" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1279,7 +1301,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25">
+    <row r="35" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1299,7 +1321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25">
+    <row r="36" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1319,7 +1341,7 @@
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
+    <row r="37" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1339,7 +1361,7 @@
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="20.25">
+    <row r="38" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1359,7 +1381,7 @@
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+    <row r="39" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1379,7 +1401,7 @@
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+    <row r="40" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1399,7 +1421,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+    <row r="41" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>

</xml_diff>